<commit_message>
core functionality finished, needs cleaning
</commit_message>
<xml_diff>
--- a/v2/placeholder_dataset_1.xlsx
+++ b/v2/placeholder_dataset_1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t xml:space="preserve">Placeholder Data</t>
   </si>
@@ -29,13 +29,13 @@
     <t xml:space="preserve">README</t>
   </si>
   <si>
-    <t xml:space="preserve">Δ[Glucose] (mg/dL)</t>
+    <t xml:space="preserve">d[Glucose]/dt (mg/dL/min)</t>
   </si>
   <si>
     <t xml:space="preserve">CA125 (U/ml)*</t>
   </si>
   <si>
-    <t xml:space="preserve">This placeholder data was created by modifying experimental results from another, unrelated experiment. Its purpose is to stand-in for characterization data for a CA125-detecting, trehlase-producing riboswitch until that data becomes available. The IV and DV columns were scaled to be within the range of normal human blood glucose levels and CA125 levels, respectively. While the shape of this distribution might be very different from what the real distribution ends up looking like, the range of the IV and DV columns should be somewhat realistic.</t>
+    <t xml:space="preserve">This placeholder data was created by modifying experimental results from another, unrelated experiment. Its purpose is to stand-in for characterization data for a CA125-detecting, trehlase-producing riboswitch until that data becomes available. The DV column was scaled to be within the range normal CA125 level. Disclaimer: the shape of this distribution may be very different from that of real-world calibration data.</t>
   </si>
   <si>
     <t xml:space="preserve">*units based on standard measurement convention. Source: https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8074643/</t>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8074643/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$'Placeholder Data'.$A$3:$A$322</t>
   </si>
   <si>
     <t xml:space="preserve">Time</t>
@@ -137,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -177,13 +180,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -306,7 +302,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -319,6 +315,18 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="0"/>
+        <b val="1"/>
+        <sz val="11"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -408,7 +416,7 @@
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:rPr>
-              <a:t>Placeholder Data: CA125 vs Δ[Glucose]</a:t>
+              <a:t>Placeholder Data: CA125 vs d[Glucose]/dt (not including +/- SD)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -488,6 +496,975 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
+              <c:f>'Placeholder Data'!$B$3:$B$322</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="320"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.124134436750549</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.24134436750549</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.35855429826043</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.30332714068569</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.63435230535383</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.62742779935822</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.95845296402635</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.8618476608681</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.91707481844283</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.94460395203513</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.94460395203513</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.1445701739571</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.6411079209593</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.31008275629117</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.0548893767945</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.6341834149637</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.1376456679615</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.6961661881439</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.0341158588076</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.1168721499747</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13.8203006248944</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14.8961324100659</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>15.4754264482351</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16.8822833980746</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>19.2822158419186</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19.6132410065867</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>22.0131734504307</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>21.8062827225131</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>23.6269211281878</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>24.9510217868603</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>28.6750548893768</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>28.0957608512076</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>32.3990879918933</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38.6058098294207</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>38.1092720824185</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41.5022800202668</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44.2332376287789</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>48.8675899341327</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>53.7502111129877</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>57.3087316331701</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>62.4809998311096</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>67.6946461746327</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>75.8875190001689</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>79.3219050836007</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>88.797500422226</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>91.1974328660699</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>99.059280526938</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>110.02448910657</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>113.996791082587</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>124.465461915217</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>126.61712548556</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>138.03749366661</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>151.402634690086</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>161.043742611045</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>169.609018746833</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>184.670663739233</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>185.787873669988</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>196.173788211451</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>201.718459719642</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>204.077014017902</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>202.504644485729</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>207.883803411586</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>211.400945786185</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>212.145752406688</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>206.973484208749</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>210.738895456849</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>219.221415301469</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>210.863029893599</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>214.545684850532</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>215.414625907786</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>212.269886843439</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>204.28390474582</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>214.669819287283</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>222.738557676068</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>212.435399425773</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>216.904239148792</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>214.75257557845</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>213.056071609525</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>215.414625907786</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>211.194055058267</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>214.8767100152</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>214.587062996116</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>212.476777571356</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>212.062996115521</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>209.787198108428</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>213.138827900692</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>214.8767100152</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>216.40770140179</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>213.800878230029</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>215.497382198953</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>223.317851714237</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>214.587062996116</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>215.456004053369</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>214.545684850532</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>214.711197432866</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>215.538760344536</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>218.766255700051</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>215.456004053369</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>215.70427292687</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>217.731802060463</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>219.924843776389</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>220.17311264989</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>221.000675561561</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>213.718121938862</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>215.58013849012</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>221.373078871812</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>218.6421212633</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>218.021449079547</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>216.490457692957</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>218.269717953048</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>217.980070933964</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>219.46968417497</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>218.559364972133</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>217.690423914879</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>225.386758993413</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>216.324945110623</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>224.393683499409</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>221.621347745313</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>218.6421212633</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>220.007600067556</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>220.628272251309</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>220.545515960142</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>220.711028542476</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>223.483364296572</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>212.311264989022</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>219.386927883803</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>224.476439790576</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>220.711028542476</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>221.57996959973</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>225.138490119912</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>219.055902719135</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>219.883465630806</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>218.849011991218</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>226.752237797669</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>224.931599391995</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>231.46934639419</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>221.828238473231</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>223.441986150988</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>225.179868265496</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>225.924674885999</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>222.366154365817</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>222.904070258402</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>226.959128525587</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>223.152339131903</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>226.793615943253</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>223.566120587739</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>224.021280189157</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>225.883296740415</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>225.924674885999</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>220.793784833643</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>222.904070258402</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>223.979902043574</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>228.614254348928</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>224.310927208242</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>228.862523222429</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>224.104036480324</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>223.11096098632</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>223.81438946124</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>221.70410403648</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>223.276473568654</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>222.904070258402</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>227.166019253505</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>230.931430501604</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>228.821145076845</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>226.297078196251</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>229.193548387097</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>228.365985475426</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>225.635027866914</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>220.297247086641</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>222.614423239318</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>228.614254348928</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>228.159094747509</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>229.855598716433</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>234.572707312954</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>228.821145076845</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>224.310927208242</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>225.179868265496</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>228.117716601925</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>230.310758317852</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>229.193548387097</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>228.779766931262</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>229.028035804763</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>225.717784158081</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>230.228002026685</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>232.545178179362</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>226.503968924168</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>226.503968924168</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>227.372909981422</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>233.165850363114</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>234.655463604121</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>228.531498057761</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>230.062489444351</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>228.490119912177</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>225.759162303665</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>232.379665597028</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>232.007262286776</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>232.090018577943</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>226.421212633001</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>229.524573551765</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>229.152170241513</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>232.007262286776</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>233.993413274785</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>231.303833811856</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>230.807296064854</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>228.572876203344</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>235.565782806958</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>230.062489444351</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>237.758824522885</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>226.090187468333</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>235.855429826043</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>234.614085458537</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>232.710690761696</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>228.365985475426</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>228.40736362101</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>228.241851038676</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>226.297078196251</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>228.821145076845</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>231.717615267691</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>227.662557000507</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>230.64178348252</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>235.648539098125</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>231.717615267691</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>229.276304678264</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>232.917581489613</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>232.379665597028</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>231.014186792771</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>234.862354332039</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>236.269211281878</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>234.738219895288</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>237.096774193548</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>229.11079209593</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>228.821145076845</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>234.738219895288</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>236.682992737713</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>232.214153014693</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>232.87620334403</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>230.352136463435</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>236.269211281878</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>230.931430501604</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>231.676237122108</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>230.600405336936</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>233.165850363114</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>235.276135787874</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>229.524573551765</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>238.793278162473</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>232.090018577943</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>232.586556324945</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>227.662557000507</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>238.462252997804</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>233.621009964533</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>232.87620334403</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>231.552102685357</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>229.483195406181</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>231.221077520689</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>230.724539773687</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>234.614085458537</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>235.689917243709</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>229.731464279682</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>228.862523222429</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>232.090018577943</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>236.682992737713</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>230.890052356021</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>232.421043742611</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>234.076169565952</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>235.317513933457</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>230.062489444351</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>232.090018577943</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>233.083094071947</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>238.751900016889</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>230.600405336936</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>230.062489444351</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>235.896807971626</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>240.862185441648</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>233.248606654281</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>230.931430501604</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>234.158925857119</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>235.069245059956</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>235.524404661375</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>237.551933794967</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>235.689917243709</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>229.23492653268</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>241.979395372403</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>240.117378821145</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>232.586556324945</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>236.434723864212</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>236.889883465631</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>235.358892079041</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>232.627934470529</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>233.414119236615</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>235.689917243709</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>233.083094071947</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>237.800202668468</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>240.365647694646</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>240.40702584023</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>237.593311940551</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>234.903732477622</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>231.262455666273</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>233.372741091032</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>240.489782131397</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>236.600236446546</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>236.682992737713</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>240.903563587232</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>238.545009288971</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>237.427799358217</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>227.952204019591</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>236.476102009796</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>239.538084782976</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>238.545009288971</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>234.820976186455</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>241.482857625401</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>229.483195406181</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>240.324269549063</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>235.648539098125</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>231.014186792771</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>234.820976186455</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>234.820976186455</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>231.510724539774</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>238.338118561054</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>'Placeholder Data'!$A$3:$A$322</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1454,983 +2431,14 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Placeholder Data'!$B$3:$B$322</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="320"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.124134436750549</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.24134436750549</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.35855429826043</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.30332714068569</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.63435230535383</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.62742779935822</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.95845296402635</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.8618476608681</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.91707481844283</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.94460395203513</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7.94460395203513</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9.1445701739571</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9.6411079209593</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9.31008275629117</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>10.0548893767945</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>10.6341834149637</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>10.1376456679615</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>13.6961661881439</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>13.0341158588076</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>13.1168721499747</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>13.8203006248944</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>14.8961324100659</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>15.4754264482351</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>16.8822833980746</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>19.2822158419186</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>19.6132410065867</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>22.0131734504307</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>21.8062827225131</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>23.6269211281878</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>24.9510217868603</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>28.6750548893768</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>28.0957608512076</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>32.3990879918933</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>38.6058098294207</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>38.1092720824185</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>41.5022800202668</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>44.2332376287789</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>48.8675899341327</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>53.7502111129877</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>57.3087316331701</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>62.4809998311096</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>67.6946461746327</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>75.8875190001689</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>79.3219050836007</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>88.797500422226</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>91.1974328660699</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>99.059280526938</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>110.02448910657</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>113.996791082587</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>124.465461915217</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>126.61712548556</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>138.03749366661</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>151.402634690086</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>161.043742611045</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>169.609018746833</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>184.670663739233</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>185.787873669988</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>196.173788211451</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>201.718459719642</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>204.077014017902</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>202.504644485729</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>207.883803411586</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>211.400945786185</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>212.145752406688</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>206.973484208749</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>210.738895456849</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>219.221415301469</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>210.863029893599</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>214.545684850532</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>215.414625907786</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>212.269886843439</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>204.28390474582</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>214.669819287283</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>222.738557676068</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>212.435399425773</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>216.904239148792</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>214.75257557845</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>213.056071609525</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>215.414625907786</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>211.194055058267</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>214.8767100152</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>214.587062996116</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>212.476777571356</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>212.062996115521</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>209.787198108428</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>213.138827900692</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>214.8767100152</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>216.40770140179</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>213.800878230029</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>215.497382198953</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>223.317851714237</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>214.587062996116</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>215.456004053369</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>214.545684850532</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>214.711197432866</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>215.538760344536</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>218.766255700051</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>215.456004053369</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>215.70427292687</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>217.731802060463</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>219.924843776389</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>220.17311264989</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>221.000675561561</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>213.718121938862</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>215.58013849012</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>221.373078871812</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>218.6421212633</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>218.021449079547</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>216.490457692957</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>218.269717953048</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>217.980070933964</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>219.46968417497</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>218.559364972133</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>217.690423914879</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>225.386758993413</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>216.324945110623</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>224.393683499409</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>221.621347745313</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>218.6421212633</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>220.007600067556</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>220.628272251309</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>220.545515960142</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>220.711028542476</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>223.483364296572</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>212.311264989022</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>219.386927883803</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>224.476439790576</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>220.711028542476</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>221.57996959973</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>225.138490119912</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>219.055902719135</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>219.883465630806</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>218.849011991218</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>226.752237797669</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>224.931599391995</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>231.46934639419</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>221.828238473231</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>223.441986150988</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>225.179868265496</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>225.924674885999</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>222.366154365817</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>222.904070258402</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>226.959128525587</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>223.152339131903</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>226.793615943253</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>223.566120587739</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>224.021280189157</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>225.883296740415</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>225.924674885999</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>220.793784833643</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>222.904070258402</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>223.979902043574</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>228.614254348928</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>224.310927208242</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>228.862523222429</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>224.104036480324</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>223.11096098632</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>223.81438946124</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>221.70410403648</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>223.276473568654</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>222.904070258402</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>227.166019253505</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>230.931430501604</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>228.821145076845</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>226.297078196251</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>229.193548387097</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>228.365985475426</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>225.635027866914</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>220.297247086641</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>222.614423239318</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>228.614254348928</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>228.159094747509</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>229.855598716433</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>234.572707312954</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>228.821145076845</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>224.310927208242</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>225.179868265496</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>228.117716601925</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>230.310758317852</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>229.193548387097</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>228.779766931262</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>229.028035804763</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>225.717784158081</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>230.228002026685</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>232.545178179362</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>226.503968924168</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>226.503968924168</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>227.372909981422</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>233.165850363114</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>234.655463604121</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>228.531498057761</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>230.062489444351</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>228.490119912177</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>225.759162303665</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>232.379665597028</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>232.007262286776</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>232.090018577943</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>226.421212633001</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>229.524573551765</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>229.152170241513</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>232.007262286776</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>233.993413274785</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>231.303833811856</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>230.807296064854</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>228.572876203344</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>235.565782806958</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>230.062489444351</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>237.758824522885</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>226.090187468333</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>235.855429826043</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>234.614085458537</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>232.710690761696</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>228.365985475426</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>228.40736362101</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>228.241851038676</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>226.297078196251</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>228.821145076845</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>231.717615267691</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>227.662557000507</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>230.64178348252</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>235.648539098125</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>231.717615267691</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>229.276304678264</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>232.917581489613</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>232.379665597028</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>231.014186792771</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>234.862354332039</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>236.269211281878</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>234.738219895288</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>237.096774193548</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>229.11079209593</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>228.821145076845</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>234.738219895288</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>236.682992737713</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>232.214153014693</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>232.87620334403</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>230.352136463435</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>236.269211281878</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>230.931430501604</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>231.676237122108</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>230.600405336936</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>233.165850363114</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>235.276135787874</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>229.524573551765</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>238.793278162473</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>232.090018577943</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>232.586556324945</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>227.662557000507</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>238.462252997804</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>233.621009964533</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>232.87620334403</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>231.552102685357</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>229.483195406181</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>231.221077520689</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>230.724539773687</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>234.614085458537</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>235.689917243709</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>229.731464279682</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>228.862523222429</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>232.090018577943</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>236.682992737713</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>230.890052356021</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>232.421043742611</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>234.076169565952</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>235.317513933457</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>230.062489444351</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>232.090018577943</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>233.083094071947</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>238.751900016889</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>230.600405336936</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>230.062489444351</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>235.896807971626</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>240.862185441648</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>233.248606654281</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>230.931430501604</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>234.158925857119</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>235.069245059956</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>235.524404661375</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>237.551933794967</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>235.689917243709</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>229.23492653268</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>241.979395372403</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>240.117378821145</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>232.586556324945</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>236.434723864212</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>236.889883465631</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>235.358892079041</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>232.627934470529</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>233.414119236615</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>235.689917243709</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>233.083094071947</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>237.800202668468</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>240.365647694646</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>240.40702584023</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>237.593311940551</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>234.903732477622</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>231.262455666273</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>233.372741091032</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>240.489782131397</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>236.600236446546</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>236.682992737713</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>240.903563587232</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>238.545009288971</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>237.427799358217</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>227.952204019591</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>236.476102009796</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>239.538084782976</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>238.545009288971</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>234.820976186455</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>241.482857625401</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>229.483195406181</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>240.324269549063</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>235.648539098125</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>231.014186792771</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>234.820976186455</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>234.820976186455</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>231.510724539774</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>238.338118561054</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="85273261"/>
-        <c:axId val="34807946"/>
+        <c:axId val="25519134"/>
+        <c:axId val="42922727"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85273261"/>
+        <c:axId val="25519134"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2467,7 +2475,7 @@
                     </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Change in Glucose Concentraion (mmol/L)</a:t>
+                  <a:t>RoC of Glucose Concentraion (mg/dL/min)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2506,12 +2514,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34807946"/>
+        <c:crossAx val="42922727"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="34807946"/>
+        <c:axId val="42922727"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2587,9 +2595,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85273261"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="25519134"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
+        <c:minorUnit val="100"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2619,16 +2628,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>83520</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>883800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>974880</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1774800</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>100800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2636,8 +2645,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4892400" y="4074480"/>
-        <a:ext cx="9093600" cy="4190040"/>
+        <a:off x="4138920" y="3837960"/>
+        <a:ext cx="9093960" cy="30620160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2827,32 +2836,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L322"/>
+  <dimension ref="A1:M322"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="13.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="24.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="13.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="24.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="28.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="G1" s="1"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -2861,16 +2877,21 @@
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="n">
@@ -2879,14 +2900,19 @@
       <c r="B3" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="4"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="25.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
@@ -2895,18 +2921,21 @@
       <c r="B4" s="6" t="n">
         <v>0.124134436750549</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="J4" s="7" t="s">
+      <c r="I4" s="4"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2917,11 +2946,17 @@
       <c r="B5" s="6" t="n">
         <v>1.24134436750549</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="n">
@@ -2930,11 +2965,17 @@
       <c r="B6" s="6" t="n">
         <v>2.35855429826043</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="0"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="n">
@@ -2943,11 +2984,17 @@
       <c r="B7" s="6" t="n">
         <v>4.30332714068569</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
@@ -2956,13 +3003,19 @@
       <c r="B8" s="6" t="n">
         <v>4.63435230535383</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
@@ -2971,17 +3024,23 @@
       <c r="B9" s="6" t="n">
         <v>5.62742779935822</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9" t="s">
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="24.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
@@ -2990,19 +3049,25 @@
       <c r="B10" s="6" t="n">
         <v>5.95845296402635</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="0"/>
+      <c r="D10" s="0"/>
+      <c r="E10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="9" t="n">
+      <c r="F10" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="F10" s="10" t="n">
+      <c r="G10" s="10" t="n">
         <v>500</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="0"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
@@ -3011,19 +3076,25 @@
       <c r="B11" s="6" t="n">
         <v>7.8618476608681</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="9" t="n">
+      <c r="F11" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="9" t="n">
+      <c r="G11" s="9" t="n">
         <v>480</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="H11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="0"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
@@ -3032,19 +3103,25 @@
       <c r="B12" s="6" t="n">
         <v>5.91707481844283</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="9" t="n">
+      <c r="F12" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="10" t="n">
+      <c r="G12" s="10" t="n">
         <v>245</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="H12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="0"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
@@ -3069,7 +3146,7 @@
       <c r="B15" s="6" t="n">
         <v>9.1445701739571</v>
       </c>
-      <c r="K15" s="1" t="n">
+      <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -3096,6 +3173,9 @@
       <c r="B18" s="6" t="n">
         <v>10.0548893767945</v>
       </c>
+      <c r="E18" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="n">
@@ -5531,16 +5611,21 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D2:H7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E2:I7"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H12:I12"/>
   </mergeCells>
+  <conditionalFormatting sqref="B4:B322">
+    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ROW(CELL("address"))-1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="*units based on standard measurement convention. Source: https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8074643/"/>
-    <hyperlink ref="J3" r:id="rId2" display="**According to https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8074643/:"/>
-    <hyperlink ref="G12" r:id="rId3" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8074643/"/>
+    <hyperlink ref="K2" r:id="rId1" display="*units based on standard measurement convention. Source: https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8074643/"/>
+    <hyperlink ref="K3" r:id="rId2" display="**According to https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8074643/:"/>
+    <hyperlink ref="H12" r:id="rId3" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8074643/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5560,7 +5645,7 @@
   </sheetPr>
   <dimension ref="A1:J321"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -5572,19 +5657,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5603,10 +5688,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5625,7 +5710,7 @@
         <v>0.124134436750549</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" s="2" t="n">
         <f aca="false">MIN($A2:$A1048576)</f>
@@ -5652,7 +5737,7 @@
         <v>1.24134436750549</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I4" s="2" t="n">
         <f aca="false">MAX($A2:$A1048576)</f>
@@ -5679,7 +5764,7 @@
         <v>2.35855429826043</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I5" s="2" t="n">
         <f aca="false">I4-I3</f>
@@ -5722,7 +5807,7 @@
         <v>4.63435230535383</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5788,7 +5873,7 @@
         <v>7.8618476608681</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>0</v>

</xml_diff>